<commit_message>
- Refactor code - Support Macro - Update Testcase.xlsx: add sheet 'Macro'
</commit_message>
<xml_diff>
--- a/testcase/Testcase.xlsx
+++ b/testcase/Testcase.xlsx
@@ -3,19 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SOURCE\SeleniumAutomationTest\testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997E9FD3-54DD-41AE-8136-6E38FC1AEE0C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80535051-A8D3-4F08-846C-D22E0DC9D20D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="506" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="506" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testcase" sheetId="5" r:id="rId1"/>
     <sheet name="Master" sheetId="3" r:id="rId2"/>
     <sheet name="Commands" sheetId="6" r:id="rId3"/>
+    <sheet name="Macro" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Testcase!$A$8:$G$11</definedName>
@@ -23,10 +24,10 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 2" guid="{6F20758C-85C0-4D64-A526-0013CC02A9C8}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 1" guid="{18E4D75C-CC47-4F6F-98E5-56578B31BB19}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Nong fillter" guid="{23DB263A-3DD3-4B16-AC22-9E5E3CAE4093}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter_H" guid="{81C1371D-BFC8-4C02-B2DE-57D9434051C9}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Nong fillter" guid="{23DB263A-3DD3-4B16-AC22-9E5E3CAE4093}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{18E4D75C-CC47-4F6F-98E5-56578B31BB19}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{6F20758C-85C0-4D64-A526-0013CC02A9C8}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="99">
   <si>
     <t>ID</t>
   </si>
@@ -334,6 +335,12 @@
   </si>
   <si>
     <t>Thoát chương trình</t>
+  </si>
+  <si>
+    <t>openGoogle</t>
+  </si>
+  <si>
+    <t>get "http://google.com"</t>
   </si>
 </sst>
 </file>
@@ -450,7 +457,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="119">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -580,827 +587,22 @@
       <diagonal/>
     </border>
     <border>
-      <bottom style="medium"/>
-    </border>
-    <border>
-      <left style="medium"/>
-      <bottom style="medium"/>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right style="medium"/>
-      <bottom style="medium"/>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-    </border>
-    <border>
-      <bottom style="medium"/>
-    </border>
-    <border>
-      <left style="medium"/>
-      <bottom style="medium"/>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right style="medium"/>
-      <bottom style="medium"/>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium">
-        <color indexed="0"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="0"/>
-      </left>
-      <right style="medium"/>
-      <top style="medium">
-        <color indexed="0"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="0"/>
-      </left>
-      <right style="medium">
+      <left/>
+      <right style="thin">
         <color indexed="0"/>
       </right>
-      <top style="medium">
-        <color indexed="0"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
+      <top/>
       <bottom style="thin">
         <color indexed="0"/>
       </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color indexed="0"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="0"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color indexed="0"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="0"/>
-      </left>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <top style="thin">
-        <color indexed="0"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="thick"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <bottom style="thick"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thick"/>
-      <bottom style="thick"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thick"/>
-      <top style="thin"/>
-      <bottom style="thick"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thick"/>
-      <top style="thin"/>
-      <bottom style="thick">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thick"/>
-      <top style="thin">
-        <color indexed="0"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="0"/>
-      </left>
-      <right style="thick"/>
-      <top style="thin">
-        <color indexed="0"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="0"/>
-      </left>
-      <right style="thick">
-        <color indexed="0"/>
-      </right>
-      <top style="thin">
-        <color indexed="0"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="thick"/>
-    </border>
-    <border>
-      <left style="thick"/>
-      <bottom style="thick"/>
-    </border>
-    <border>
-      <left style="thick"/>
-      <right style="thick"/>
-      <bottom style="thick"/>
-    </border>
-    <border>
-      <left style="thick"/>
-      <right style="thick"/>
-      <top style="thick"/>
-      <bottom style="thick"/>
-    </border>
-    <border>
-      <left style="thick"/>
-      <right style="thick"/>
-      <top style="thick"/>
-      <bottom style="thick">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thick"/>
-      <right style="thick"/>
-      <top style="thick">
-        <color indexed="0"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="0"/>
-      </left>
-      <right style="thick"/>
-      <top style="thick">
-        <color indexed="0"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="0"/>
-      </left>
-      <right style="thick">
-        <color indexed="0"/>
-      </right>
-      <top style="thick">
-        <color indexed="0"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color indexed="0"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="0"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color indexed="0"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="0"/>
-      </left>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <top style="thin">
-        <color indexed="0"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thick"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thick"/>
-      <top style="thick"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thick"/>
-      <top style="thick"/>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thick"/>
-      <top style="thick">
-        <color indexed="0"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="0"/>
-      </left>
-      <right style="thick"/>
-      <top style="thick">
-        <color indexed="0"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="0"/>
-      </left>
-      <right style="thick">
-        <color indexed="0"/>
-      </right>
-      <top style="thick">
-        <color indexed="0"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thick"/>
-    </border>
-    <border>
-      <right style="thick"/>
-      <top style="thick"/>
-    </border>
-    <border>
-      <right style="thick"/>
-      <top style="thick"/>
-      <bottom>
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thick"/>
-      <top style="thick">
-        <color indexed="0"/>
-      </top>
-      <bottom>
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="0"/>
-      </left>
-      <right style="thick"/>
-      <top style="thick">
-        <color indexed="0"/>
-      </top>
-      <bottom>
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="0"/>
-      </left>
-      <right style="thick">
-        <color indexed="0"/>
-      </right>
-      <top style="thick">
-        <color indexed="0"/>
-      </top>
-      <bottom>
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin"/>
-    </border>
-    <border>
-      <right style="thin"/>
-      <top style="thin"/>
-    </border>
-    <border>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom>
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin"/>
-      <top style="thin">
-        <color indexed="0"/>
-      </top>
-      <bottom>
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <top style="thin">
-        <color indexed="0"/>
-      </top>
-      <bottom>
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <right style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <right style="thin"/>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <right style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <right style="thin"/>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="0"/>
-      </left>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="0"/>
-      </left>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <top>
-        <color indexed="0"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <right style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <right style="thin"/>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="0"/>
-      </left>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="0"/>
-      </left>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <top>
-        <color indexed="0"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <right style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <right style="thin"/>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="0"/>
-      </left>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="0"/>
-      </left>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <top>
-        <color indexed="0"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <right style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <right style="thin"/>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="0"/>
-      </left>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="0"/>
-      </left>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <top>
-        <color indexed="0"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <right style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <right style="thin"/>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="0"/>
-      </left>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="0"/>
-      </left>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <top>
-        <color indexed="0"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <right style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <right style="thin"/>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="0"/>
-      </left>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="0"/>
-      </left>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <top>
-        <color indexed="0"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <right style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <right style="thin"/>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="0"/>
-      </left>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="0"/>
-      </left>
-      <right style="thin">
-        <color indexed="0"/>
-      </right>
-      <top>
-        <color indexed="0"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="0"/>
-      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1489,35 +691,8 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="7" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="82" xfId="0" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="88" xfId="0" applyBorder="true">
-      <alignment shrinkToFit="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="94" xfId="0" applyBorder="true">
-      <alignment shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="100" xfId="0" applyBorder="true">
-      <alignment wrapText="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="106" xfId="0" applyBorder="true">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="112" xfId="0" applyBorder="true">
-      <alignment shrinkToFit="false" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="118" xfId="0" applyBorder="true">
-      <alignment shrinkToFit="true" wrapText="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1871,13 +1046,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="24" width="49.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="36.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="29.42578125" collapsed="true"/>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="49" style="24" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="36.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
@@ -7650,15 +6825,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="26.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="35.7109375" collapsed="true"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="35.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
@@ -7677,257 +6852,284 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s" s="55">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="B4" t="s" s="55">
+      <c r="B4" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="C4" t="s" s="55">
+      <c r="C4" s="38" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s" s="55">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="B5" t="s" s="55">
+      <c r="B5" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="C5" t="s" s="55">
+      <c r="C5" s="38" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s" s="55">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="B6" t="s" s="55">
+      <c r="B6" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C6" t="s" s="55">
+      <c r="C6" s="38" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="s" s="55">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B7" t="s" s="55">
+      <c r="B7" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C7" t="s" s="55">
+      <c r="C7" s="38" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s" s="55">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="B8" t="s" s="55">
+      <c r="B8" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="C8" t="s" s="55">
+      <c r="C8" s="38" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="s" s="55">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="B9" t="s" s="55">
+      <c r="B9" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C9" t="s" s="55">
+      <c r="C9" s="38" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="s" s="55">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="B10" t="s" s="55">
+      <c r="B10" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C10" t="s" s="55">
+      <c r="C10" s="38" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="s" s="55">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="B11" t="s" s="55">
+      <c r="B11" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C11" t="s" s="55">
+      <c r="C11" s="38" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="s" s="55">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="B12" t="s" s="55">
+      <c r="B12" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C12" t="s" s="55">
+      <c r="C12" s="38" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="s" s="55">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="B13" t="s" s="55">
+      <c r="B13" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="C13" t="s" s="55">
+      <c r="C13" s="38" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="s" s="55">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="B14" t="s" s="55">
+      <c r="B14" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="C14" t="s" s="55">
+      <c r="C14" s="38" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="s" s="55">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="B15" t="s" s="55">
+      <c r="B15" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="C15" t="s" s="55">
+      <c r="C15" s="38" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="s" s="55">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="B16" t="s" s="55">
+      <c r="B16" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="C16" t="s" s="55">
+      <c r="C16" s="38" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="s" s="55">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="B17" t="s" s="55">
+      <c r="B17" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C17" t="s" s="55">
+      <c r="C17" s="38" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="s" s="55">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="B18" t="s" s="55">
+      <c r="B18" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C18" t="s" s="55">
+      <c r="C18" s="38" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="s" s="55">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="B19" t="s" s="55">
+      <c r="B19" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C19" t="s" s="55">
+      <c r="C19" s="38" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="s" s="55">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="B20" t="s" s="55">
+      <c r="B20" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C20" t="s" s="55">
+      <c r="C20" s="38" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="s" s="55">
+    <row r="21" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A21" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="B21" t="s" s="55">
+      <c r="B21" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="C21" t="s" s="55">
+      <c r="C21" s="38" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="s" s="55">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="B22" t="s" s="55">
+      <c r="B22" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C22" t="s" s="55">
+      <c r="C22" s="38" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="s" s="55">
+    <row r="23" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A23" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="B23" t="s" s="55">
+      <c r="B23" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="C23" t="s" s="55">
+      <c r="C23" s="38" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="s" s="55">
+    <row r="24" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="B24" t="s" s="55">
+      <c r="B24" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="C24" t="s" s="55">
+      <c r="C24" s="38" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="s" s="55">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="B25" t="s" s="55">
+      <c r="B25" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="C25" t="s" s="55">
+      <c r="C25" s="38" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="s" s="55">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="B26" t="s" s="55">
+      <c r="B26" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="C26" t="s" s="55">
+      <c r="C26" s="38" t="s">
         <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42C51FC9-88AA-4BA7-8AFA-1D4D674AF779}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="52.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>